<commit_message>
Data driven testing framework changes.. adding test status to the excel.
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testData.xlsx
+++ b/src/test/resources/testData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Mini\Project\src\test\resources\testData\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -60,12 +60,16 @@
   </si>
   <si>
     <t xml:space="preserve">Invalid email id or Password </t>
+  </si>
+  <si>
+    <t>PASSED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,11 +434,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.7265625" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
-    <col min="3" max="3" width="26.54296875" customWidth="1"/>
-    <col min="4" max="4" width="24.7265625" customWidth="1"/>
-    <col min="5" max="5" width="25.54296875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="51.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.1796875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.54296875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.7265625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.54296875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -464,6 +468,9 @@
       <c r="C2">
         <v>1234</v>
       </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -477,6 +484,9 @@
       </c>
       <c r="D3" t="s">
         <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
My Cart test cases added.
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testData.xlsx
+++ b/src/test/resources/testData/testData.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Mini\Project\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEDE884-A933-4DAD-B8F0-10062FA491FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F0602B-5854-437E-B3D9-633FEDD10C1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6E156075-8B2B-4F49-8691-DB610BF91AFE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{6E156075-8B2B-4F49-8691-DB610BF91AFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="MyCart" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -63,14 +64,52 @@
   </si>
   <si>
     <t>PASSED</t>
+  </si>
+  <si>
+    <t>Test Case Description</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Shipping Address</t>
+  </si>
+  <si>
+    <t>Billing Address</t>
+  </si>
+  <si>
+    <t>TC_SC_001 - Add to Cart</t>
+  </si>
+  <si>
+    <t>TC_SC_015 -  Choose Payment Methods</t>
+  </si>
+  <si>
+    <t>TC_SC_016 - Proceed to checkout</t>
+  </si>
+  <si>
+    <t>TC_SC_017 - navigating to the track orders - by clicking on the Track button of the order history page.</t>
+  </si>
+  <si>
+    <t>123, address villa, address road :  Western : Colombo : 11100</t>
+  </si>
+  <si>
+    <t>123, address villa, address road :  Western : Colombo : 11101</t>
+  </si>
+  <si>
+    <t>123, address villa, address road :  Western : Colombo : 11102</t>
+  </si>
+  <si>
+    <t>123, address villa, address road :  Western : Colombo : 11103</t>
+  </si>
+  <si>
+    <t>Test Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +121,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,9 +153,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -428,17 +479,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C31778B-0D08-41C3-8A02-CEED05F62F3B}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="51.7265625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.54296875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.7265625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="25.54296875" collapsed="true"/>
+    <col min="1" max="1" width="51.7265625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.7265625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -496,4 +547,121 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62159897-7643-4E41-90C6-48B78680E32C}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="35.6328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.7265625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.36328125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1234</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1234</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1234</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1234</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F120450D-682E-422B-84A2-EA3C52F96F6C}"/>
+    <hyperlink ref="B3:B5" r:id="rId2" display="test@user.com" xr:uid="{75026836-664A-4DF0-A353-8C74F0198750}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed by thihari 05/06
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testData.xlsx
+++ b/src/test/resources/testData/testData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Mini\FinalProject\UiAutomationForOnlineShoppingSite\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini Project V2\UiAutomationForOnlineShoppingSite\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C35150-6E27-4064-A6CA-64710A488A4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A5430E-175D-40BB-9E76-6B2991AE2CF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="933" activeTab="9" xr2:uid="{6E156075-8B2B-4F49-8691-DB610BF91AFE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="933" firstSheet="1" activeTab="1" xr2:uid="{6E156075-8B2B-4F49-8691-DB610BF91AFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="108">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -268,9 +268,6 @@
   </si>
   <si>
     <t>Bill Smith</t>
-  </si>
-  <si>
-    <t>bill@gmail.com</t>
   </si>
   <si>
     <t>077234567890</t>
@@ -368,6 +365,12 @@
   </si>
   <si>
     <t>0112123123</t>
+  </si>
+  <si>
+    <t>billabc@gmail.com</t>
+  </si>
+  <si>
+    <t>0112123126</t>
   </si>
 </sst>
 </file>
@@ -866,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9797AD85-75EB-4524-BFFB-D669ABC9ED66}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C5"/>
     </sheetView>
   </sheetViews>
@@ -926,7 +929,7 @@
         <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -943,7 +946,7 @@
         <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -960,7 +963,7 @@
         <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1006,7 +1009,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="B2:C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1052,40 +1055,40 @@
         <v>73</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
         <v>69</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>41</v>
@@ -1096,20 +1099,20 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>41</v>
@@ -1120,20 +1123,20 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>41</v>
@@ -1144,20 +1147,20 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>41</v>
@@ -1168,19 +1171,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
@@ -1192,25 +1195,25 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" s="4">
         <v>1234567</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H8" t="s">
         <v>7</v>
@@ -1264,16 +1267,16 @@
     </row>
     <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
         <v>65</v>
@@ -1310,10 +1313,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>60</v>
@@ -1324,7 +1327,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="4">
         <v>8</v>
@@ -1341,7 +1344,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -1350,7 +1353,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -1358,7 +1361,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="4">
         <v>8</v>
@@ -1367,7 +1370,7 @@
         <v>69</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -1375,7 +1378,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
@@ -1384,7 +1387,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -1406,7 +1409,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1428,7 +1431,7 @@
         <v>59</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -1451,7 +1454,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="4">
         <v>1234</v>
@@ -1460,7 +1463,7 @@
         <v>1234</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -1468,13 +1471,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="4">
         <v>1234</v>
@@ -1483,7 +1486,7 @@
         <v>1234</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -1491,13 +1494,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D4" s="4">
         <v>1234</v>
@@ -1506,7 +1509,7 @@
         <v>1234</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
         <v>65</v>
@@ -1514,11 +1517,11 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="4">
         <v>1234</v>
@@ -1535,7 +1538,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>6</v>
@@ -1569,7 +1572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62159897-7643-4E41-90C6-48B78680E32C}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1784,7 +1787,7 @@
         <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1844,7 +1847,7 @@
         <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1852,16 +1855,16 @@
         <v>38</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1873,7 +1876,7 @@
         <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1881,13 +1884,13 @@
         <v>42</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F5" t="s">
         <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1948,7 +1951,7 @@
         <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2012,7 +2015,7 @@
         <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed by thihari(f) 05/06
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testData.xlsx
+++ b/src/test/resources/testData/testData.xlsx
@@ -5,18 +5,30 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Mini\Project\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini Project V2\UiAutomationForOnlineShoppingSite\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F0602B-5854-437E-B3D9-633FEDD10C1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED4982B-F677-4634-B2F1-33FEC4B531EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{6E156075-8B2B-4F49-8691-DB610BF91AFE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="933" firstSheet="2" activeTab="9" xr2:uid="{6E156075-8B2B-4F49-8691-DB610BF91AFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="MyCart" sheetId="3" r:id="rId2"/>
+    <sheet name="Search" sheetId="9" r:id="rId3"/>
+    <sheet name="Change Password" sheetId="10" r:id="rId4"/>
+    <sheet name="My Profile" sheetId="11" r:id="rId5"/>
+    <sheet name="Billing Address" sheetId="12" r:id="rId6"/>
+    <sheet name="Shipping Address" sheetId="13" r:id="rId7"/>
+    <sheet name="Order History" sheetId="14" r:id="rId8"/>
+    <sheet name="Payment Pending Order" sheetId="15" r:id="rId9"/>
+    <sheet name="LoginData" sheetId="4" r:id="rId10"/>
+    <sheet name="SignUpData" sheetId="5" r:id="rId11"/>
+    <sheet name="HomeData" sheetId="6" r:id="rId12"/>
+    <sheet name="TrackOrder" sheetId="7" r:id="rId13"/>
+    <sheet name="ForgotPW" sheetId="8" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="108">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -51,10 +63,13 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Login in with valid username and password</t>
+  </si>
+  <si>
     <t>test@user.com</t>
   </si>
   <si>
-    <t>Login in with valid username and password</t>
+    <t>PASSED</t>
   </si>
   <si>
     <t>Login in with valid username and invalid password</t>
@@ -63,53 +78,306 @@
     <t xml:space="preserve">Invalid email id or Password </t>
   </si>
   <si>
-    <t>PASSED</t>
-  </si>
-  <si>
     <t>Test Case Description</t>
   </si>
   <si>
     <t>User Name</t>
   </si>
   <si>
+    <t>Billing Address</t>
+  </si>
+  <si>
     <t>Shipping Address</t>
   </si>
   <si>
-    <t>Billing Address</t>
+    <t>Test Status</t>
   </si>
   <si>
     <t>TC_SC_001 - Add to Cart</t>
   </si>
   <si>
+    <t>123, address villa, address road :  Western : Colombo : 11100</t>
+  </si>
+  <si>
     <t>TC_SC_015 -  Choose Payment Methods</t>
   </si>
   <si>
+    <t>123, address villa, address road :  Western : Colombo : 11101</t>
+  </si>
+  <si>
     <t>TC_SC_016 - Proceed to checkout</t>
   </si>
   <si>
+    <t>123, address villa, address road :  Western : Colombo : 11102</t>
+  </si>
+  <si>
     <t>TC_SC_017 - navigating to the track orders - by clicking on the Track button of the order history page.</t>
   </si>
   <si>
-    <t>123, address villa, address road :  Western : Colombo : 11100</t>
-  </si>
-  <si>
-    <t>123, address villa, address road :  Western : Colombo : 11101</t>
-  </si>
-  <si>
-    <t>123, address villa, address road :  Western : Colombo : 11102</t>
-  </si>
-  <si>
     <t>123, address villa, address road :  Western : Colombo : 11103</t>
   </si>
   <si>
-    <t>Test Status</t>
+    <t>Search field</t>
+  </si>
+  <si>
+    <t>Search Product</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>Invalid Search Product</t>
+  </si>
+  <si>
+    <t>Current Password</t>
+  </si>
+  <si>
+    <t>New Password</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>Alert Message</t>
+  </si>
+  <si>
+    <t>Update with current password, new password and confirm password</t>
+  </si>
+  <si>
+    <t>Password Changed Successfully !!</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Contact No</t>
+  </si>
+  <si>
+    <t>Page Title</t>
+  </si>
+  <si>
+    <t>Verify page Title</t>
+  </si>
+  <si>
+    <t>My Account</t>
+  </si>
+  <si>
+    <t>Update with valid name and contact no</t>
+  </si>
+  <si>
+    <t>Your info has been updated</t>
+  </si>
+  <si>
+    <t>Update with empty name and empty contact no</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
+  </si>
+  <si>
+    <t>Update with empty name and contact no</t>
+  </si>
+  <si>
+    <t>Billing State</t>
+  </si>
+  <si>
+    <t>Billing City</t>
+  </si>
+  <si>
+    <t>Billing Pincode</t>
+  </si>
+  <si>
+    <t>Update with valid values for mandatory fields</t>
+  </si>
+  <si>
+    <t>No 87/P/5, Colombo 7</t>
+  </si>
+  <si>
+    <t>Colombo</t>
+  </si>
+  <si>
+    <t>Billing Address has been updated</t>
+  </si>
+  <si>
+    <t>Shipping State</t>
+  </si>
+  <si>
+    <t>Shipping City</t>
+  </si>
+  <si>
+    <t>Shipping Pincode</t>
+  </si>
+  <si>
+    <t>No 38/C, Galle</t>
+  </si>
+  <si>
+    <t>Galle</t>
+  </si>
+  <si>
+    <t>Shipping Address has been updated</t>
+  </si>
+  <si>
+    <t>Verify page title</t>
+  </si>
+  <si>
+    <t>Order History</t>
+  </si>
+  <si>
+    <t>Pending Order History</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Error Message</t>
+  </si>
+  <si>
+    <t>Valid email address &amp; password</t>
+  </si>
+  <si>
+    <t>Valid email address &amp; invalid password</t>
+  </si>
+  <si>
+    <t>Invalid email id or Password</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>Inalid email address &amp; valid password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid email aaddress &amp; invalid password </t>
+  </si>
+  <si>
+    <t>lkjhgfds</t>
+  </si>
+  <si>
+    <t>tvs@gmail.com</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Contact number</t>
+  </si>
+  <si>
+    <t>All valid fields</t>
+  </si>
+  <si>
+    <t>Bill Smith</t>
+  </si>
+  <si>
+    <t>077234567890</t>
+  </si>
+  <si>
+    <t>abcdefg</t>
+  </si>
+  <si>
+    <t>You are successfully register</t>
+  </si>
+  <si>
+    <t>Empty full name with valid other fields</t>
+  </si>
+  <si>
+    <t>077234567891</t>
+  </si>
+  <si>
+    <t>Empty email address with valid other fields</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
+    <t>Empty contact no with valid other fields</t>
+  </si>
+  <si>
+    <t>harry@gmail.com</t>
+  </si>
+  <si>
+    <t>Empty password with valid other fields</t>
+  </si>
+  <si>
+    <t>Empty confirm password with valid other fields</t>
+  </si>
+  <si>
+    <t>Different confirmation password with valid other fields</t>
+  </si>
+  <si>
+    <t>Password and Confirm Password Field do not match  !!</t>
+  </si>
+  <si>
+    <t>successfully logout function verification</t>
+  </si>
+  <si>
+    <t>You have successfully logout</t>
+  </si>
+  <si>
+    <t>Order Id</t>
+  </si>
+  <si>
+    <t>Registered Email</t>
+  </si>
+  <si>
+    <t>Valid Order Id &amp; valid email</t>
+  </si>
+  <si>
+    <t>Invalid Order Id &amp; valid email</t>
+  </si>
+  <si>
+    <t>Either order id or Registered email id is invalid</t>
+  </si>
+  <si>
+    <t>Valid Order Id &amp; invalid email</t>
+  </si>
+  <si>
+    <t>Inalid Order Id &amp; invalid email</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Password Changed Successfully</t>
+  </si>
+  <si>
+    <t>Invalid email address</t>
+  </si>
+  <si>
+    <t>Invalid email id or Contact no</t>
+  </si>
+  <si>
+    <t>Invalid contact number</t>
+  </si>
+  <si>
+    <t>Empty email address</t>
+  </si>
+  <si>
+    <t>Empty contact number</t>
+  </si>
+  <si>
+    <t>dhimatestnew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234
+</t>
+  </si>
+  <si>
+    <t>0112123123</t>
+  </si>
+  <si>
+    <t>0112123128</t>
+  </si>
+  <si>
+    <t>billabcd@gmail.com</t>
+  </si>
+  <si>
+    <t>Welcome -dhimatestnew</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +395,26 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,7 +441,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -162,6 +450,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -511,33 +827,33 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C2">
         <v>1234</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>12345567788</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -549,9 +865,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62159897-7643-4E41-90C6-48B78680E32C}">
-  <dimension ref="A1:F5"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9797AD85-75EB-4524-BFFB-D669ABC9ED66}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -559,13 +875,699 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.6328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="31.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="33.7265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.36328125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="30" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1234</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1234</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{436FD121-E15D-455B-9658-A9329607C709}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{94157DA8-F52A-40F3-9A27-3008DB93FDB1}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{1EBAF953-0D08-4BAA-B89D-5673A9A222EE}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{BC281D22-32EA-4D99-925F-1EAA81D4341B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8714B825-9F64-480B-9A9E-31F2D422379D}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="49.81640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.90625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.36328125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.08984375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.36328125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1234567</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{0D096DAB-C622-499B-A8A5-74C12C6CF35C}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{4B6E6EC2-C007-4D6C-AE33-56AB3D1457A6}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{D26130E3-BD5D-4C98-852F-29083F9D920F}"/>
+    <hyperlink ref="C6:C8" r:id="rId4" display="harry@gmail.com" xr:uid="{AA180983-364E-44AB-B0F2-1531BC041179}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D5D583-6B99-4CC7-B39E-430FDCC24B19}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37.453125" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.26953125" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.54296875" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.54296875" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.453125" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="8.7265625" style="4" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{1BC71C72-A0D5-4BC3-9499-4DC9E7514793}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C63BAE-EA2E-47FB-865B-6CFB8E1E6EDE}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.1796875" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.81640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.7265625" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.1796875" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="8.7265625" style="4" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="4">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="4">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{5CC04A92-6DA2-4235-AA1E-A928D0BB95D4}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{EA155C92-A106-4E1A-8C2C-BE1CCCFC8F4E}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{744B84E3-58AC-4A0A-A9F9-79A9EA6E1FB2}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{F6DD1577-91CD-4F24-9DDF-1B542E91F490}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A16AB4-9685-4599-A406-D48B2A182784}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.54296875" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.54296875" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.54296875" style="7" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.453125" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.81640625" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.7265625" style="4" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1234</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1234</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1234</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1234</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1234</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1234</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1234</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1234</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1234</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1234</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B11" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{4751E19D-4B4B-417A-9572-C7BAAB9DB60E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62159897-7643-4E41-90C6-48B78680E32C}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="35.54296875" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.453125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.26953125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7265625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="33.7265625" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.453125" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.7265625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -579,55 +1581,61 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
         <v>1234</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>1234</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>1234</v>
@@ -641,19 +1649,19 @@
     </row>
     <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>1234</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -664,4 +1672,419 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61C39E0-B9AB-4F5F-A3F5-41F00791B579}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="10">
+        <v>1234</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF13A1DF-3AAF-4A65-B7C1-84D5D7F564E5}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="50.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.26953125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="23.1796875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="C2">
+        <v>1234</v>
+      </c>
+      <c r="D2">
+        <v>1234</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="abc123@#" xr:uid="{7EC849F1-E7D3-4FEF-ABA8-EE3F4E791088}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD2D4640-601D-4CC5-9A09-1A153D889E8A}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="45.81640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.453125" style="15" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.26953125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD9AEF2-04EA-42F9-A0B5-211322CBB090}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2">
+        <v>10123</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="abc123@#" xr:uid="{6DA4F95C-1A20-4412-B481-CCA01260714F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07CAD8BD-E7FD-4904-AE9A-D67FAE5B5BED}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2">
+        <v>335</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="abc123@#" xr:uid="{812ECCA8-F3DB-4AE4-9445-BCFC61BC7A2E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD09D9A6-398F-4B28-BB3B-9FC3D3C30D62}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4359984C-1892-4497-B7CB-5B91E4F062E3}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed by Dhimanshi(Final) 06/06
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testData.xlsx
+++ b/src/test/resources/testData/testData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini Project V2\UiAutomationForOnlineShoppingSite\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fresher Traning Program - Technical QE Track Training\Mini Project V2.0\UiAutomationForOnlineShoppingSite\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED4982B-F677-4634-B2F1-33FEC4B531EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44947177-9A3C-4984-B5F8-35B59CB9070F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="933" firstSheet="2" activeTab="9" xr2:uid="{6E156075-8B2B-4F49-8691-DB610BF91AFE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="933" firstSheet="4" activeTab="13" xr2:uid="{6E156075-8B2B-4F49-8691-DB610BF91AFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="104">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -100,21 +100,6 @@
   </si>
   <si>
     <t>TC_SC_015 -  Choose Payment Methods</t>
-  </si>
-  <si>
-    <t>123, address villa, address road :  Western : Colombo : 11101</t>
-  </si>
-  <si>
-    <t>TC_SC_016 - Proceed to checkout</t>
-  </si>
-  <si>
-    <t>123, address villa, address road :  Western : Colombo : 11102</t>
-  </si>
-  <si>
-    <t>TC_SC_017 - navigating to the track orders - by clicking on the Track button of the order history page.</t>
-  </si>
-  <si>
-    <t>123, address villa, address road :  Western : Colombo : 11103</t>
   </si>
   <si>
     <t>Search field</t>
@@ -364,19 +349,23 @@
     <t>0112123123</t>
   </si>
   <si>
-    <t>0112123128</t>
-  </si>
-  <si>
     <t>billabcd@gmail.com</t>
   </si>
   <si>
     <t>Welcome -dhimatestnew</t>
+  </si>
+  <si>
+    <t>TC_SC_002 - Add single item to the shopping cart</t>
+  </si>
+  <si>
+    <t>TC_SC_004 - Add single item, multiple times to the shopping cart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -801,11 +790,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.7265625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.54296875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.7265625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.54296875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="51.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.1796875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.54296875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.7265625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.54296875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -869,16 +858,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9797AD85-75EB-4524-BFFB-D669ABC9ED66}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.26953125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="30" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.54296875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.26953125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="30.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -886,13 +875,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
@@ -900,7 +889,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -909,24 +898,24 @@
         <v>1234</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -934,16 +923,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C4" s="4">
         <v>1234</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -951,16 +940,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -992,16 +981,16 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.90625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.36328125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.08984375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.36328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="49.81640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.36328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.08984375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1009,22 +998,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>4</v>
@@ -1032,49 +1021,49 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
         <v>7</v>
@@ -1082,23 +1071,23 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
         <v>7</v>
@@ -1106,23 +1095,23 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
         <v>7</v>
@@ -1130,23 +1119,23 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
         <v>7</v>
@@ -1154,23 +1143,23 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
         <v>7</v>
@@ -1178,25 +1167,25 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F8" s="4">
         <v>1234567</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H8" t="s">
         <v>7</v>
@@ -1223,12 +1212,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.453125" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.26953125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.54296875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.54296875" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.453125" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="8.7265625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="37.453125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="16.26953125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="14.54296875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="26.54296875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="16.453125" collapsed="true"/>
+    <col min="6" max="16384" style="4" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1236,13 +1225,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
@@ -1250,19 +1239,19 @@
     </row>
     <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1283,12 +1272,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.81640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.7265625" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.1796875" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="8.7265625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="27.1796875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="18.81640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="17.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="20.7265625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="19.1796875" collapsed="true"/>
+    <col min="6" max="16384" style="4" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1296,13 +1285,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
@@ -1310,7 +1299,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B2" s="4">
         <v>8</v>
@@ -1319,7 +1308,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -1327,7 +1316,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -1336,7 +1325,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -1344,16 +1333,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B4" s="4">
         <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -1361,16 +1350,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -1391,19 +1380,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A16AB4-9685-4599-A406-D48B2A182784}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.54296875" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.54296875" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.54296875" style="7" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.453125" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.81640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="8.7265625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="32.54296875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="17.54296875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="7" width="18.54296875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="17.453125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="17.81640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="32.0" collapsed="true"/>
+    <col min="7" max="16384" style="4" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1411,19 +1400,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>4</v>
@@ -1431,13 +1420,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D2" s="4">
         <v>1234</v>
@@ -1446,7 +1435,7 @@
         <v>1234</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -1454,13 +1443,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D3" s="4">
         <v>1234</v>
@@ -1469,7 +1458,7 @@
         <v>1234</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -1477,13 +1466,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D4" s="4">
         <v>1234</v>
@@ -1492,19 +1481,19 @@
         <v>1234</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D5" s="4">
         <v>1234</v>
@@ -1513,7 +1502,7 @@
         <v>1234</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
@@ -1521,7 +1510,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>6</v>
@@ -1533,7 +1522,7 @@
         <v>1234</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
@@ -1556,18 +1545,18 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.453125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.26953125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.7265625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33.7265625" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.453125" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="8.7265625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="35.54296875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="23.453125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="16.26953125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="31.7265625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="33.7265625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="26.453125" collapsed="true"/>
+    <col min="7" max="16384" style="2" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -1610,65 +1599,34 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1234</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="F3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1234</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1234</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B5" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F120450D-682E-422B-84A2-EA3C52F96F6C}"/>
-    <hyperlink ref="B3:B5" r:id="rId2" display="test@user.com" xr:uid="{75026836-664A-4DF0-A353-8C74F0198750}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1689,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>4</v>
@@ -1697,10 +1655,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>7</v>
@@ -1708,7 +1666,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B3" s="10">
         <v>1234</v>
@@ -1732,11 +1690,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.26953125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.81640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.26953125" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="23.1796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="50.453125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.26953125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.81640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.26953125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="23.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -1744,16 +1702,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1761,7 +1719,7 @@
     </row>
     <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B2" s="11">
         <v>1234</v>
@@ -1773,7 +1731,7 @@
         <v>1234</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -1797,12 +1755,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.81640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.453125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.453125" style="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.54296875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.26953125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.81640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.453125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="15" width="22.453125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.26953125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1810,16 +1768,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1830,10 +1788,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -1841,16 +1799,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -1858,11 +1816,11 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B4" s="13"/>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
@@ -1870,13 +1828,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
@@ -1905,16 +1863,16 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1922,22 +1880,22 @@
     </row>
     <row r="2" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>10123</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -1969,16 +1927,16 @@
         <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1986,22 +1944,22 @@
     </row>
     <row r="2" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <v>335</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -2030,7 +1988,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -2038,10 +1996,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -2067,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -2075,10 +2033,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>

</xml_diff>